<commit_message>
add the mssql and maria db files
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\defsecone project\DSEC360-\backend\DSEC\scan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\1_dsec\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DE8524-3DF2-44BC-8065-825BD0CA9305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEA193A-736F-43A2-A125-7F750539B3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Categories</t>
   </si>
@@ -54,15 +54,6 @@
     <t>Ubuntu_Linux_24.04_LTS_Benchmark_v1.0.0</t>
   </si>
   <si>
-    <t>Microsoft SQL Server 2019 Benchmark v1.5.0</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server 2017 Benchmark v1.3.0</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server 2016 Benchmark v1.4.0</t>
-  </si>
-  <si>
     <t>Microsoft_Windows_10_Stand-alone_v3.0.0</t>
   </si>
   <si>
@@ -91,6 +82,27 @@
   </si>
   <si>
     <t>Oracle</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server 2019</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server 2017</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server 2016</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server 2022</t>
+  </si>
+  <si>
+    <t>MARIA</t>
+  </si>
+  <si>
+    <t>MariaDB 10_11</t>
+  </si>
+  <si>
+    <t>MariaDB 10_6</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,10 +442,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -444,13 +456,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -458,13 +470,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -472,10 +484,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -489,10 +501,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -503,10 +515,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -517,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
@@ -531,12 +543,54 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change os to windows
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\1_dsec\DSEC360-\backend\DSEC\scan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEA193A-736F-43A2-A125-7F750539B3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EACA82-DF7D-4C02-A4A3-E8BEAAFDF6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Categories</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>MariaDB 10_6</t>
+  </si>
+  <si>
+    <t>Windows</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +459,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -470,7 +473,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
changed the connection function for the mssql
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\1_dsec\DSEC360-\backend\DSEC\scan\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20E7BCC4-D8D8-45A9-82B4-3B95CC445521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">=Sheet1!$A$1:$A$67</definedName>
-  </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -64,9 +68,6 @@
     <t>ORACLE</t>
   </si>
   <si>
-    <t>Oracle</t>
-  </si>
-  <si>
     <t>MSSQL</t>
   </si>
   <si>
@@ -89,13 +90,15 @@
   </si>
   <si>
     <t>MariaDB 10_6</t>
+  </si>
+  <si>
+    <t>Oracle 12C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,23 +128,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -152,10 +152,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -193,71 +193,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -285,7 +285,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -308,11 +308,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -321,13 +321,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -337,7 +337,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -346,7 +346,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -355,7 +355,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -363,10 +363,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -431,187 +431,188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Suse and Redhat
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\1_dsec\DSEC360-\backend\DSEC\scan\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20E7BCC4-D8D8-45A9-82B4-3B95CC445521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>Configuration Name</t>
   </si>
@@ -59,6 +52,12 @@
     <t>Debian Linux 12</t>
   </si>
   <si>
+    <t>Redhat_9</t>
+  </si>
+  <si>
+    <t>Suse_15</t>
+  </si>
+  <si>
     <t>Ubuntu Linux 24.04</t>
   </si>
   <si>
@@ -68,6 +67,9 @@
     <t>ORACLE</t>
   </si>
   <si>
+    <t>Oracle 12C</t>
+  </si>
+  <si>
     <t>MSSQL</t>
   </si>
   <si>
@@ -90,15 +92,13 @@
   </si>
   <si>
     <t>MariaDB 10_6</t>
-  </si>
-  <si>
-    <t>Oracle 12C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,20 +128,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -152,10 +155,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -193,71 +196,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -285,7 +288,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -308,11 +311,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -321,13 +324,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -337,7 +340,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -346,7 +349,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -355,7 +358,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -363,10 +366,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -431,188 +434,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="37.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="37.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="15.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remodal of result page
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\defsecone project\DSEC360-\backend\DSEC\scan\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B40E735-7A57-4AA0-A945-F988E5A725F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Configuration Name</t>
   </si>
@@ -100,8 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,23 +136,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -158,10 +160,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -199,71 +201,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -291,7 +293,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -314,11 +316,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -327,13 +329,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -343,7 +345,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -352,7 +354,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -361,7 +363,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -369,10 +371,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -437,227 +439,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1" t="s">
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1" t="s">
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
impleted remote access for fortigate firewall
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit - Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\defsecone project\DSEC360-\backend\DSEC\scan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\1_dsec\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B40E735-7A57-4AA0-A945-F988E5A725F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6010BE55-45E8-4820-8A2C-8C5A122C2075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Configuration Name</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>MariaDB 10_6</t>
+  </si>
+  <si>
+    <t>FORTIGATE</t>
+  </si>
+  <si>
+    <t>PALOALTO</t>
+  </si>
+  <si>
+    <t>Fortigate 7.0</t>
+  </si>
+  <si>
+    <t>Firewall</t>
+  </si>
+  <si>
+    <t>palo</t>
   </si>
 </sst>
 </file>
@@ -443,10 +458,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,6 +681,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>